<commit_message>
chore: - update dependencies; - fix `read_xl_to_db_test.rs`
</commit_message>
<xml_diff>
--- a/mock/test2.xlsx
+++ b/mock/test2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18110" windowHeight="11990"/>
+    <workbookView windowWidth="15530" windowHeight="25730"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>first_name</t>
+  </si>
+  <si>
+    <t>int</t>
   </si>
   <si>
     <t>num</t>
@@ -54,8 +57,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -68,6 +71,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,42 +94,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,17 +130,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -165,14 +176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -191,7 +194,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,13 +210,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,31 +224,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,43 +380,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,13 +392,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,85 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,21 +445,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -467,6 +455,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,6 +486,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -503,25 +515,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -530,16 +533,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,16 +551,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -569,100 +569,103 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="11"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="11" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -982,15 +985,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1003,61 +1006,76 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
+        <v>0.82</v>
+      </c>
+      <c r="D2" s="1">
         <v>0.9</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>11</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
+        <v>1.01</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.8</v>
       </c>
-      <c r="D3" t="s">
-        <v>7</v>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
+        <v>1.37</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.9</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
+      <c r="E4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
+        <v>0.94</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.7</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>